<commit_message>
Update before farm mods
</commit_message>
<xml_diff>
--- a/input_Farm_English.xlsx
+++ b/input_Farm_English.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\excel translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE09D3F-6C55-4BF2-B29D-453F80996CF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA085C0-0CF3-45A0-8F4E-02CFE525CFBA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="380" windowWidth="18930" windowHeight="9800" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KAWASAKI CDW _プログラム6桁_Tコン V" sheetId="21" r:id="rId1"/>
@@ -674,7 +674,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="801">
   <si>
     <t>J/E</t>
   </si>
@@ -2296,12 +2296,6 @@
     <t>Enter WS: 0, CC: Same number as Gun Number, OC: O (Release)</t>
   </si>
   <si>
-    <t>If the hammering device has been ON for a set period of time,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> it is considered "OK".</t>
-  </si>
-  <si>
     <t>In the case of NG, the line will stop for weld abnormality</t>
   </si>
   <si>
@@ -3199,12 +3193,6 @@
     <t>2nd start position, jump to Work Pro</t>
   </si>
   <si>
-    <t>※* For stationary use, use the stabilizing tool before</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> supplying work to the gun.</t>
-  </si>
-  <si>
     <t>Matehan motor brake lock command</t>
   </si>
   <si>
@@ -3212,6 +3200,12 @@
   </si>
   <si>
     <t>Operation Diagram</t>
+  </si>
+  <si>
+    <t>※* For stationary use, use the stabilizing tool before supplying work to the gun.</t>
+  </si>
+  <si>
+    <t>If the hammering device has been ON for a set period of time, it is considered "OK".</t>
   </si>
 </sst>
 </file>
@@ -16130,8 +16124,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5054745" y="29701837"/>
-          <a:ext cx="5429642" cy="8261464"/>
+          <a:off x="5126182" y="30133637"/>
+          <a:ext cx="5537592" cy="8393226"/>
           <a:chOff x="13542818" y="44092091"/>
           <a:chExt cx="6374637" cy="8295091"/>
         </a:xfrm>
@@ -16300,8 +16294,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="36698122" y="4399643"/>
-          <a:ext cx="1815372" cy="1803514"/>
+          <a:off x="37368047" y="4431393"/>
+          <a:ext cx="1791559" cy="1827326"/>
           <a:chOff x="38741689" y="6561535"/>
           <a:chExt cx="1944201" cy="1211774"/>
         </a:xfrm>
@@ -16430,8 +16424,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="36793286" y="7939088"/>
-          <a:ext cx="1761154" cy="1340303"/>
+          <a:off x="37463211" y="8026400"/>
+          <a:ext cx="1730991" cy="1356178"/>
           <a:chOff x="38741689" y="6561536"/>
           <a:chExt cx="1944181" cy="900545"/>
         </a:xfrm>
@@ -18241,8 +18235,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="37242750" y="13787439"/>
-          <a:ext cx="1836452" cy="1000125"/>
+          <a:off x="37893625" y="13970001"/>
+          <a:ext cx="1828514" cy="1016000"/>
           <a:chOff x="38741689" y="6561536"/>
           <a:chExt cx="1944187" cy="900545"/>
         </a:xfrm>
@@ -18371,8 +18365,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="38894548" y="22354601"/>
-          <a:ext cx="1814443" cy="889663"/>
+          <a:off x="39540660" y="22675276"/>
+          <a:ext cx="1816031" cy="894425"/>
           <a:chOff x="38741688" y="6910741"/>
           <a:chExt cx="1832663" cy="576633"/>
         </a:xfrm>
@@ -18501,8 +18495,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="38925651" y="23400119"/>
-          <a:ext cx="1956310" cy="1801012"/>
+          <a:off x="39568588" y="23733494"/>
+          <a:ext cx="1961073" cy="1821649"/>
           <a:chOff x="38741687" y="6727381"/>
           <a:chExt cx="1967608" cy="1170238"/>
         </a:xfrm>
@@ -18631,8 +18625,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6242050" y="15608826"/>
-          <a:ext cx="14726832" cy="3400550"/>
+          <a:off x="6342062" y="15815201"/>
+          <a:ext cx="15076082" cy="3459287"/>
           <a:chOff x="10382233" y="5996770"/>
           <a:chExt cx="15274520" cy="3405122"/>
         </a:xfrm>
@@ -19676,8 +19670,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="36793278" y="36442650"/>
-          <a:ext cx="1761159" cy="1340303"/>
+          <a:off x="37463203" y="36982400"/>
+          <a:ext cx="1730996" cy="1356178"/>
           <a:chOff x="38741689" y="6561536"/>
           <a:chExt cx="1944187" cy="900545"/>
         </a:xfrm>
@@ -20022,8 +20016,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="37230050" y="15832139"/>
-          <a:ext cx="1798352" cy="1404936"/>
+          <a:off x="37893625" y="16049626"/>
+          <a:ext cx="1780889" cy="1420811"/>
           <a:chOff x="38741689" y="6561536"/>
           <a:chExt cx="1944187" cy="900545"/>
         </a:xfrm>
@@ -21976,8 +21970,8 @@
   </sheetPr>
   <dimension ref="B2:BH84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:AT4"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="AA28" zoomScale="40" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="AW38" sqref="AW38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -22028,7 +22022,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="AV2" s="232" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="2:60" ht="14.25" customHeight="1" thickTop="1">
@@ -22039,7 +22033,7 @@
     <row r="4" spans="2:60" ht="75" customHeight="1">
       <c r="B4" s="214"/>
       <c r="C4" s="243" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="D4" s="244"/>
       <c r="E4" s="244"/>
@@ -22085,7 +22079,7 @@
       <c r="AS4" s="244"/>
       <c r="AT4" s="244"/>
       <c r="AU4" s="245" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="AV4" s="246"/>
       <c r="AW4" s="246"/>
@@ -22281,31 +22275,31 @@
       <c r="AT7" s="7"/>
       <c r="AU7" s="9"/>
       <c r="AV7" s="20" t="s">
+        <v>515</v>
+      </c>
+      <c r="AW7" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="AX7" s="21" t="s">
+        <v>516</v>
+      </c>
+      <c r="AY7" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="AW7" s="21" t="s">
+      <c r="AZ7" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="BA7" s="21" t="s">
+        <v>519</v>
+      </c>
+      <c r="BB7" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="BC7" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="BD7" s="21" t="s">
         <v>524</v>
-      </c>
-      <c r="AX7" s="21" t="s">
-        <v>518</v>
-      </c>
-      <c r="AY7" s="21" t="s">
-        <v>519</v>
-      </c>
-      <c r="AZ7" s="21" t="s">
-        <v>520</v>
-      </c>
-      <c r="BA7" s="21" t="s">
-        <v>521</v>
-      </c>
-      <c r="BB7" s="21" t="s">
-        <v>522</v>
-      </c>
-      <c r="BC7" s="21" t="s">
-        <v>523</v>
-      </c>
-      <c r="BD7" s="21" t="s">
-        <v>526</v>
       </c>
       <c r="BE7" s="21" t="s">
         <v>0</v>
@@ -22317,7 +22311,7 @@
         <v>2</v>
       </c>
       <c r="BH7" s="195" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" spans="2:60" ht="40" customHeight="1">
@@ -22371,7 +22365,7 @@
         <v>1</v>
       </c>
       <c r="AW8" s="51" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="AX8" s="52"/>
       <c r="AY8" s="53"/>
@@ -22380,13 +22374,13 @@
       <c r="BB8" s="53"/>
       <c r="BC8" s="53"/>
       <c r="BD8" s="53" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="BE8" s="53"/>
       <c r="BF8" s="54"/>
       <c r="BG8" s="54"/>
       <c r="BH8" s="196" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="9" spans="2:60" ht="40" customHeight="1">
@@ -22451,13 +22445,13 @@
       <c r="BB9" s="53"/>
       <c r="BC9" s="53"/>
       <c r="BD9" s="53" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="BE9" s="53"/>
       <c r="BF9" s="54"/>
       <c r="BG9" s="54"/>
       <c r="BH9" s="197" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="10" spans="2:60" ht="40" customHeight="1">
@@ -22534,7 +22528,7 @@
       </c>
       <c r="BG10" s="32"/>
       <c r="BH10" s="197" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="11" spans="2:60" ht="40" customHeight="1">
@@ -22611,7 +22605,7 @@
         <v>479</v>
       </c>
       <c r="BH11" s="198" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="12" spans="2:60" ht="40" customHeight="1">
@@ -22688,7 +22682,7 @@
       </c>
       <c r="BG12" s="54"/>
       <c r="BH12" s="198" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13" spans="2:60" ht="40" customHeight="1">
@@ -22767,7 +22761,7 @@
         <v>48124</v>
       </c>
       <c r="BH13" s="257" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="14" spans="2:60" ht="40" customHeight="1">
@@ -22917,7 +22911,7 @@
       <c r="BF15" s="63"/>
       <c r="BG15" s="28"/>
       <c r="BH15" s="199" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="16" spans="2:60" ht="40" customHeight="1">
@@ -23067,7 +23061,7 @@
       </c>
       <c r="BG17" s="28"/>
       <c r="BH17" s="196" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="18" spans="2:60" ht="40" customHeight="1">
@@ -23146,7 +23140,7 @@
         <v>64</v>
       </c>
       <c r="BH18" s="251" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="19" spans="2:60" ht="40" customHeight="1">
@@ -23644,31 +23638,31 @@
       <c r="AT26" s="14"/>
       <c r="AU26" s="254"/>
       <c r="AV26" s="20" t="s">
+        <v>515</v>
+      </c>
+      <c r="AW26" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="AX26" s="21" t="s">
+        <v>516</v>
+      </c>
+      <c r="AY26" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="AW26" s="21" t="s">
+      <c r="AZ26" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="BA26" s="21" t="s">
+        <v>519</v>
+      </c>
+      <c r="BB26" s="21" t="s">
+        <v>520</v>
+      </c>
+      <c r="BC26" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="BD26" s="21" t="s">
         <v>524</v>
-      </c>
-      <c r="AX26" s="21" t="s">
-        <v>518</v>
-      </c>
-      <c r="AY26" s="21" t="s">
-        <v>519</v>
-      </c>
-      <c r="AZ26" s="21" t="s">
-        <v>520</v>
-      </c>
-      <c r="BA26" s="21" t="s">
-        <v>521</v>
-      </c>
-      <c r="BB26" s="21" t="s">
-        <v>522</v>
-      </c>
-      <c r="BC26" s="21" t="s">
-        <v>523</v>
-      </c>
-      <c r="BD26" s="21" t="s">
-        <v>526</v>
       </c>
       <c r="BE26" s="21" t="s">
         <v>0</v>
@@ -23680,7 +23674,7 @@
         <v>2</v>
       </c>
       <c r="BH26" s="195" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27" spans="2:60" ht="40" customHeight="1">
@@ -23734,7 +23728,7 @@
         <v>1</v>
       </c>
       <c r="AW27" s="78" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="AX27" s="79"/>
       <c r="AY27" s="80"/>
@@ -23743,7 +23737,7 @@
       <c r="BB27" s="80"/>
       <c r="BC27" s="80"/>
       <c r="BD27" s="80" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="BE27" s="81"/>
       <c r="BF27" s="82"/>
@@ -23810,13 +23804,13 @@
       <c r="BB28" s="80"/>
       <c r="BC28" s="80"/>
       <c r="BD28" s="80" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="BE28" s="83"/>
       <c r="BF28" s="84"/>
       <c r="BG28" s="40"/>
       <c r="BH28" s="258" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="29" spans="2:60" ht="40" customHeight="1">
@@ -24035,7 +24029,7 @@
       <c r="BF31" s="92"/>
       <c r="BG31" s="92"/>
       <c r="BH31" s="238" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="32" spans="2:60" ht="40" customHeight="1">
@@ -24089,7 +24083,7 @@
         <v>6</v>
       </c>
       <c r="AW32" s="94" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AX32" s="95"/>
       <c r="AY32" s="96"/>
@@ -24181,7 +24175,7 @@
         <v>65</v>
       </c>
       <c r="BH33" s="39" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="34" spans="2:60" ht="40" customHeight="1">
@@ -24248,7 +24242,7 @@
       <c r="BF34" s="92"/>
       <c r="BG34" s="92"/>
       <c r="BH34" s="238" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="35" spans="2:60" ht="40" customHeight="1">
@@ -24329,7 +24323,7 @@
         <v>169</v>
       </c>
       <c r="BH35" s="212" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="36" spans="2:60" ht="40" customHeight="1">
@@ -24396,7 +24390,7 @@
       <c r="BF36" s="92"/>
       <c r="BG36" s="92"/>
       <c r="BH36" s="238" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="37" spans="2:60" ht="40" customHeight="1">
@@ -24448,7 +24442,7 @@
       <c r="AU37" s="254"/>
       <c r="AV37" s="106"/>
       <c r="AW37" s="37" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="AY37" s="34"/>
       <c r="AZ37" s="34"/>
@@ -24509,9 +24503,7 @@
       <c r="AT38" s="14"/>
       <c r="AU38" s="254"/>
       <c r="AV38" s="92"/>
-      <c r="AW38" s="37" t="s">
-        <v>799</v>
-      </c>
+      <c r="AW38" s="37"/>
       <c r="AX38" s="92"/>
       <c r="AY38" s="92"/>
       <c r="AZ38" s="92"/>
@@ -24785,7 +24777,7 @@
       <c r="BF42" s="129"/>
       <c r="BG42" s="92"/>
       <c r="BH42" s="130" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="43" spans="2:60" ht="40" customHeight="1">
@@ -24870,7 +24862,7 @@
       </c>
       <c r="BG43" s="108"/>
       <c r="BH43" s="131" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="44" spans="2:60" ht="40" customHeight="1">
@@ -24953,7 +24945,7 @@
         <v>482</v>
       </c>
       <c r="BH44" s="38" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="45" spans="2:60" ht="40" customHeight="1">
@@ -25034,7 +25026,7 @@
         <v>472</v>
       </c>
       <c r="BH45" s="111" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="46" spans="2:60" ht="40" customHeight="1">
@@ -25113,7 +25105,7 @@
       <c r="BF46" s="107"/>
       <c r="BG46" s="38"/>
       <c r="BH46" s="38" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="47" spans="2:60" ht="40" customHeight="1">
@@ -25194,7 +25186,7 @@
         <v>472</v>
       </c>
       <c r="BH47" s="111" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="48" spans="2:60" ht="40" customHeight="1">
@@ -25273,7 +25265,7 @@
       </c>
       <c r="BG48" s="115"/>
       <c r="BH48" s="38" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="49" spans="2:60" ht="40" customHeight="1">
@@ -25354,7 +25346,7 @@
         <v>123</v>
       </c>
       <c r="BH49" s="38" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="50" spans="2:60" ht="40" customHeight="1">
@@ -25433,7 +25425,7 @@
       </c>
       <c r="BG50" s="108"/>
       <c r="BH50" s="38" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="51" spans="2:60" ht="40" customHeight="1">
@@ -25514,7 +25506,7 @@
         <v>124</v>
       </c>
       <c r="BH51" s="38" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="52" spans="2:60" ht="40" customHeight="1">
@@ -26008,7 +26000,7 @@
     <row r="60" spans="2:60" ht="40" customHeight="1">
       <c r="B60" s="253"/>
       <c r="AG60" s="230" t="s">
-        <v>512</v>
+        <v>800</v>
       </c>
       <c r="AU60" s="254"/>
       <c r="AV60" s="99"/>
@@ -26052,7 +26044,7 @@
       <c r="AD61" s="13"/>
       <c r="AE61" s="13"/>
       <c r="AG61" s="230" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AU61" s="254"/>
       <c r="AV61" s="99">
@@ -26109,9 +26101,6 @@
       <c r="AC62" s="13"/>
       <c r="AD62" s="13"/>
       <c r="AE62" s="13"/>
-      <c r="AG62" s="230" t="s">
-        <v>514</v>
-      </c>
       <c r="AU62" s="254"/>
       <c r="AV62" s="99">
         <v>23</v>
@@ -26226,7 +26215,7 @@
         <v>24</v>
       </c>
       <c r="AW64" s="222" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="AX64" s="215"/>
       <c r="AY64" s="97"/>
@@ -26307,7 +26296,7 @@
       </c>
       <c r="BG65" s="108"/>
       <c r="BH65" s="38" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="66" spans="2:60" ht="40" customHeight="1">
@@ -26686,7 +26675,7 @@
         <v>27</v>
       </c>
       <c r="AW72" s="116" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="AX72" s="101"/>
       <c r="AY72" s="102"/>
@@ -26767,7 +26756,7 @@
       </c>
       <c r="BG73" s="121"/>
       <c r="BH73" s="105" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="74" spans="2:60" ht="40" customHeight="1">
@@ -26835,7 +26824,7 @@
       </c>
       <c r="BG74" s="38"/>
       <c r="BH74" s="38" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="75" spans="2:60" ht="40" customHeight="1">
@@ -26903,7 +26892,7 @@
         <v>64</v>
       </c>
       <c r="BH75" s="256" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="76" spans="2:60" ht="40" customHeight="1">
@@ -27233,7 +27222,7 @@
       <c r="P2" s="259"/>
       <c r="Q2" s="140"/>
       <c r="R2" s="260" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S2" s="260"/>
       <c r="T2" s="260"/>
@@ -27259,18 +27248,18 @@
     </row>
     <row r="3" spans="2:36" ht="21">
       <c r="B3" s="139" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C3" s="143"/>
       <c r="N3" s="240" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="R3" s="240"/>
       <c r="S3" s="239"/>
       <c r="T3" s="239"/>
       <c r="U3" s="239"/>
       <c r="V3" s="261" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="W3" s="261"/>
       <c r="X3" s="261"/>
@@ -27305,17 +27294,17 @@
     </row>
     <row r="5" spans="2:36" ht="16" thickBot="1">
       <c r="B5" s="262" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C5" s="262"/>
       <c r="D5" s="262"/>
       <c r="E5" s="263" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F5" s="263"/>
       <c r="G5" s="263"/>
       <c r="H5" s="264" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I5" s="264"/>
       <c r="J5" s="264"/>
@@ -27329,17 +27318,17 @@
       </c>
       <c r="Q5" s="265"/>
       <c r="R5" s="262" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="S5" s="262"/>
       <c r="T5" s="262"/>
       <c r="U5" s="263" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="V5" s="263"/>
       <c r="W5" s="263"/>
       <c r="X5" s="264" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="Y5" s="264"/>
       <c r="Z5" s="264"/>
@@ -27363,7 +27352,7 @@
       <c r="F6" s="267"/>
       <c r="G6" s="267"/>
       <c r="H6" s="268" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I6" s="269"/>
       <c r="J6" s="269"/>
@@ -27403,7 +27392,7 @@
       <c r="F7" s="287"/>
       <c r="G7" s="287"/>
       <c r="H7" s="288" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I7" s="289"/>
       <c r="J7" s="289"/>
@@ -27639,7 +27628,7 @@
     </row>
     <row r="14" spans="2:36" s="150" customFormat="1" ht="16" thickBot="1">
       <c r="B14" s="147" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C14" s="147"/>
       <c r="D14" s="147"/>
@@ -27663,7 +27652,7 @@
       <c r="V14" s="149"/>
       <c r="AE14" s="151"/>
       <c r="AF14" s="148" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="AJ14" s="152"/>
     </row>
@@ -27671,64 +27660,64 @@
       <c r="C15" s="153"/>
       <c r="D15" s="154"/>
       <c r="E15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F15" s="156"/>
       <c r="G15" s="154"/>
       <c r="H15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I15" s="156"/>
       <c r="J15" s="154"/>
       <c r="K15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="L15" s="156"/>
       <c r="M15" s="154"/>
       <c r="N15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="O15" s="156"/>
       <c r="P15" s="154"/>
       <c r="Q15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="R15" s="156"/>
       <c r="S15" s="154"/>
       <c r="T15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="U15" s="156"/>
       <c r="V15" s="154"/>
       <c r="W15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="X15" s="156"/>
       <c r="Y15" s="154"/>
       <c r="Z15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AA15" s="156"/>
       <c r="AB15" s="154"/>
       <c r="AC15" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AD15" s="156"/>
       <c r="AE15" s="154"/>
       <c r="AF15" s="242" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" spans="2:36" s="150" customFormat="1" ht="16" thickBot="1">
       <c r="C16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D16" s="158"/>
       <c r="E16" s="159" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="G16" s="158"/>
       <c r="H16" s="160" t="str">
@@ -27736,7 +27725,7 @@
         <v>R1</v>
       </c>
       <c r="I16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="J16" s="158"/>
       <c r="K16" s="160" t="str">
@@ -27744,7 +27733,7 @@
         <v>R1</v>
       </c>
       <c r="L16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M16" s="158"/>
       <c r="N16" s="160" t="str">
@@ -27752,7 +27741,7 @@
         <v>R1</v>
       </c>
       <c r="O16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="P16" s="158"/>
       <c r="Q16" s="160" t="str">
@@ -27760,7 +27749,7 @@
         <v>R1</v>
       </c>
       <c r="R16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="S16" s="158"/>
       <c r="T16" s="160" t="str">
@@ -27768,7 +27757,7 @@
         <v>R1</v>
       </c>
       <c r="U16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="V16" s="158"/>
       <c r="W16" s="160" t="str">
@@ -27776,7 +27765,7 @@
         <v>R1</v>
       </c>
       <c r="X16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="Y16" s="158"/>
       <c r="Z16" s="160" t="str">
@@ -27784,7 +27773,7 @@
         <v>R1</v>
       </c>
       <c r="AA16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AB16" s="158"/>
       <c r="AC16" s="160" t="str">
@@ -27792,7 +27781,7 @@
         <v>R1</v>
       </c>
       <c r="AD16" s="157" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AE16" s="158"/>
       <c r="AF16" s="161" t="str">
@@ -28554,7 +28543,7 @@
     </row>
     <row r="28" spans="2:33" s="146" customFormat="1">
       <c r="B28" s="146" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D28" s="166"/>
       <c r="E28" s="166"/>
@@ -28587,10 +28576,10 @@
     </row>
     <row r="29" spans="2:33">
       <c r="B29" s="233" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C29" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D29" s="310"/>
       <c r="E29" s="310"/>
@@ -28599,10 +28588,10 @@
       <c r="H29" s="310"/>
       <c r="I29" s="310"/>
       <c r="J29" s="235" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="K29" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="L29" s="310"/>
       <c r="M29" s="310"/>
@@ -28611,10 +28600,10 @@
       <c r="P29" s="310"/>
       <c r="Q29" s="310"/>
       <c r="R29" s="235" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="S29" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="T29" s="310"/>
       <c r="U29" s="310"/>
@@ -28623,10 +28612,10 @@
       <c r="X29" s="310"/>
       <c r="Y29" s="310"/>
       <c r="Z29" s="235" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="AA29" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="AB29" s="310"/>
       <c r="AC29" s="310"/>
@@ -28640,7 +28629,7 @@
         <v>109</v>
       </c>
       <c r="C30" s="317" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D30" s="317"/>
       <c r="E30" s="317"/>
@@ -28678,7 +28667,7 @@
         <v>110</v>
       </c>
       <c r="C31" s="312" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="D31" s="312"/>
       <c r="E31" s="312"/>
@@ -28690,7 +28679,7 @@
         <v>111</v>
       </c>
       <c r="K31" s="312" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="L31" s="312"/>
       <c r="M31" s="312"/>
@@ -28702,7 +28691,7 @@
         <v>112</v>
       </c>
       <c r="S31" s="320" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="T31" s="320"/>
       <c r="U31" s="320"/>
@@ -28714,7 +28703,7 @@
         <v>113</v>
       </c>
       <c r="AA31" s="312" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="AB31" s="312"/>
       <c r="AC31" s="312"/>
@@ -28728,7 +28717,7 @@
         <v>114</v>
       </c>
       <c r="C32" s="312" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D32" s="313"/>
       <c r="E32" s="313"/>
@@ -28740,7 +28729,7 @@
         <v>115</v>
       </c>
       <c r="K32" s="312" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="L32" s="312"/>
       <c r="M32" s="312"/>
@@ -28752,7 +28741,7 @@
         <v>116</v>
       </c>
       <c r="S32" s="314" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="T32" s="315"/>
       <c r="U32" s="315"/>
@@ -28764,7 +28753,7 @@
         <v>117</v>
       </c>
       <c r="AA32" s="312" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AB32" s="312"/>
       <c r="AC32" s="312"/>
@@ -28778,7 +28767,7 @@
         <v>118</v>
       </c>
       <c r="C33" s="312" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D33" s="313"/>
       <c r="E33" s="313"/>
@@ -28790,7 +28779,7 @@
         <v>119</v>
       </c>
       <c r="K33" s="312" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="L33" s="312"/>
       <c r="M33" s="312"/>
@@ -28802,7 +28791,7 @@
         <v>120</v>
       </c>
       <c r="S33" s="314" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="T33" s="315"/>
       <c r="U33" s="315"/>
@@ -28814,7 +28803,7 @@
         <v>121</v>
       </c>
       <c r="AA33" s="312" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="AB33" s="312"/>
       <c r="AC33" s="312"/>
@@ -28828,7 +28817,7 @@
         <v>122</v>
       </c>
       <c r="C34" s="312" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D34" s="313"/>
       <c r="E34" s="313"/>
@@ -28840,7 +28829,7 @@
         <v>123</v>
       </c>
       <c r="K34" s="312" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="L34" s="312"/>
       <c r="M34" s="312"/>
@@ -28852,7 +28841,7 @@
         <v>124</v>
       </c>
       <c r="S34" s="314" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="T34" s="315"/>
       <c r="U34" s="315"/>
@@ -28864,7 +28853,7 @@
         <v>125</v>
       </c>
       <c r="AA34" s="312" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="AB34" s="312"/>
       <c r="AC34" s="312"/>
@@ -28878,7 +28867,7 @@
         <v>126</v>
       </c>
       <c r="C35" s="312" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D35" s="313"/>
       <c r="E35" s="313"/>
@@ -28890,7 +28879,7 @@
         <v>127</v>
       </c>
       <c r="K35" s="312" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="L35" s="312"/>
       <c r="M35" s="312"/>
@@ -28902,7 +28891,7 @@
         <v>128</v>
       </c>
       <c r="S35" s="314" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="T35" s="315"/>
       <c r="U35" s="315"/>
@@ -28914,7 +28903,7 @@
         <v>129</v>
       </c>
       <c r="AA35" s="312" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="AB35" s="312"/>
       <c r="AC35" s="312"/>
@@ -28928,7 +28917,7 @@
         <v>130</v>
       </c>
       <c r="C36" s="321" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D36" s="322"/>
       <c r="E36" s="322"/>
@@ -28940,7 +28929,7 @@
         <v>131</v>
       </c>
       <c r="K36" s="312" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L36" s="312"/>
       <c r="M36" s="312"/>
@@ -28952,7 +28941,7 @@
         <v>132</v>
       </c>
       <c r="S36" s="323" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="T36" s="323"/>
       <c r="U36" s="323"/>
@@ -28964,7 +28953,7 @@
         <v>133</v>
       </c>
       <c r="AA36" s="312" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AB36" s="312"/>
       <c r="AC36" s="312"/>
@@ -28978,7 +28967,7 @@
         <v>134</v>
       </c>
       <c r="C37" s="324" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D37" s="325"/>
       <c r="E37" s="325"/>
@@ -28990,7 +28979,7 @@
         <v>135</v>
       </c>
       <c r="K37" s="312" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="L37" s="312"/>
       <c r="M37" s="312"/>
@@ -29012,7 +29001,7 @@
         <v>137</v>
       </c>
       <c r="AA37" s="312" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="AB37" s="312"/>
       <c r="AC37" s="312"/>
@@ -29026,7 +29015,7 @@
         <v>138</v>
       </c>
       <c r="C38" s="327" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D38" s="328"/>
       <c r="E38" s="328"/>
@@ -29038,7 +29027,7 @@
         <v>139</v>
       </c>
       <c r="K38" s="312" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="L38" s="312"/>
       <c r="M38" s="312"/>
@@ -29050,7 +29039,7 @@
         <v>140</v>
       </c>
       <c r="S38" s="320" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="T38" s="320"/>
       <c r="U38" s="320"/>
@@ -29062,7 +29051,7 @@
         <v>141</v>
       </c>
       <c r="AA38" s="312" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AB38" s="312"/>
       <c r="AC38" s="312"/>
@@ -29076,7 +29065,7 @@
         <v>142</v>
       </c>
       <c r="C39" s="327" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D39" s="328"/>
       <c r="E39" s="328"/>
@@ -29088,7 +29077,7 @@
         <v>143</v>
       </c>
       <c r="K39" s="312" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="L39" s="312"/>
       <c r="M39" s="312"/>
@@ -29100,7 +29089,7 @@
         <v>144</v>
       </c>
       <c r="S39" s="320" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="T39" s="320"/>
       <c r="U39" s="320"/>
@@ -29112,7 +29101,7 @@
         <v>145</v>
       </c>
       <c r="AA39" s="312" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="AB39" s="312"/>
       <c r="AC39" s="312"/>
@@ -29126,7 +29115,7 @@
         <v>146</v>
       </c>
       <c r="C40" s="327" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D40" s="328"/>
       <c r="E40" s="328"/>
@@ -29138,7 +29127,7 @@
         <v>147</v>
       </c>
       <c r="K40" s="312" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L40" s="312"/>
       <c r="M40" s="312"/>
@@ -29150,7 +29139,7 @@
         <v>148</v>
       </c>
       <c r="S40" s="320" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="T40" s="320"/>
       <c r="U40" s="320"/>
@@ -29162,7 +29151,7 @@
         <v>149</v>
       </c>
       <c r="AA40" s="312" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="AB40" s="312"/>
       <c r="AC40" s="312"/>
@@ -29176,7 +29165,7 @@
         <v>150</v>
       </c>
       <c r="C41" s="327" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D41" s="328"/>
       <c r="E41" s="328"/>
@@ -29188,7 +29177,7 @@
         <v>151</v>
       </c>
       <c r="K41" s="312" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L41" s="312"/>
       <c r="M41" s="312"/>
@@ -29200,7 +29189,7 @@
         <v>152</v>
       </c>
       <c r="S41" s="320" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="T41" s="320"/>
       <c r="U41" s="320"/>
@@ -29212,7 +29201,7 @@
         <v>153</v>
       </c>
       <c r="AA41" s="312" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="AB41" s="312"/>
       <c r="AC41" s="312"/>
@@ -29226,7 +29215,7 @@
         <v>154</v>
       </c>
       <c r="C42" s="327" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D42" s="328"/>
       <c r="E42" s="328"/>
@@ -29238,7 +29227,7 @@
         <v>155</v>
       </c>
       <c r="K42" s="312" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L42" s="312"/>
       <c r="M42" s="312"/>
@@ -29250,7 +29239,7 @@
         <v>156</v>
       </c>
       <c r="S42" s="320" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="T42" s="320"/>
       <c r="U42" s="320"/>
@@ -29262,7 +29251,7 @@
         <v>157</v>
       </c>
       <c r="AA42" s="312" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="AB42" s="312"/>
       <c r="AC42" s="312"/>
@@ -29276,7 +29265,7 @@
         <v>158</v>
       </c>
       <c r="C43" s="327" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D43" s="328"/>
       <c r="E43" s="328"/>
@@ -29288,7 +29277,7 @@
         <v>159</v>
       </c>
       <c r="K43" s="312" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L43" s="312"/>
       <c r="M43" s="312"/>
@@ -29300,7 +29289,7 @@
         <v>160</v>
       </c>
       <c r="S43" s="314" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="T43" s="315"/>
       <c r="U43" s="315"/>
@@ -29312,7 +29301,7 @@
         <v>161</v>
       </c>
       <c r="AA43" s="312" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="AB43" s="312"/>
       <c r="AC43" s="312"/>
@@ -29326,7 +29315,7 @@
         <v>162</v>
       </c>
       <c r="C44" s="312" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D44" s="312"/>
       <c r="E44" s="312"/>
@@ -29338,7 +29327,7 @@
         <v>163</v>
       </c>
       <c r="K44" s="312" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L44" s="312"/>
       <c r="M44" s="312"/>
@@ -29350,7 +29339,7 @@
         <v>164</v>
       </c>
       <c r="S44" s="312" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="T44" s="312"/>
       <c r="U44" s="312"/>
@@ -29362,7 +29351,7 @@
         <v>165</v>
       </c>
       <c r="AA44" s="312" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="AB44" s="312"/>
       <c r="AC44" s="312"/>
@@ -29376,7 +29365,7 @@
         <v>166</v>
       </c>
       <c r="C45" s="312" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D45" s="312"/>
       <c r="E45" s="312"/>
@@ -29388,7 +29377,7 @@
         <v>167</v>
       </c>
       <c r="K45" s="312" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L45" s="312"/>
       <c r="M45" s="312"/>
@@ -29400,7 +29389,7 @@
         <v>168</v>
       </c>
       <c r="S45" s="312" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="T45" s="312"/>
       <c r="U45" s="312"/>
@@ -29412,7 +29401,7 @@
         <v>169</v>
       </c>
       <c r="AA45" s="312" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="AB45" s="312"/>
       <c r="AC45" s="312"/>
@@ -29426,7 +29415,7 @@
         <v>170</v>
       </c>
       <c r="C46" s="312" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D46" s="312"/>
       <c r="E46" s="312"/>
@@ -29438,7 +29427,7 @@
         <v>171</v>
       </c>
       <c r="K46" s="312" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="L46" s="312"/>
       <c r="M46" s="312"/>
@@ -29450,7 +29439,7 @@
         <v>172</v>
       </c>
       <c r="S46" s="312" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="T46" s="312"/>
       <c r="U46" s="312"/>
@@ -29462,7 +29451,7 @@
         <v>173</v>
       </c>
       <c r="AA46" s="312" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="AB46" s="312"/>
       <c r="AC46" s="312"/>
@@ -29476,7 +29465,7 @@
         <v>174</v>
       </c>
       <c r="C47" s="312" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D47" s="312"/>
       <c r="E47" s="312"/>
@@ -29488,7 +29477,7 @@
         <v>175</v>
       </c>
       <c r="K47" s="312" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L47" s="312"/>
       <c r="M47" s="312"/>
@@ -29500,7 +29489,7 @@
         <v>176</v>
       </c>
       <c r="S47" s="312" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="T47" s="312"/>
       <c r="U47" s="312"/>
@@ -29512,7 +29501,7 @@
         <v>177</v>
       </c>
       <c r="AA47" s="312" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="AB47" s="312"/>
       <c r="AC47" s="312"/>
@@ -29526,7 +29515,7 @@
         <v>178</v>
       </c>
       <c r="C48" s="312" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D48" s="328"/>
       <c r="E48" s="328"/>
@@ -29538,7 +29527,7 @@
         <v>179</v>
       </c>
       <c r="K48" s="312" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="L48" s="312"/>
       <c r="M48" s="312"/>
@@ -29550,7 +29539,7 @@
         <v>180</v>
       </c>
       <c r="S48" s="312" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="T48" s="328"/>
       <c r="U48" s="328"/>
@@ -29562,7 +29551,7 @@
         <v>181</v>
       </c>
       <c r="AA48" s="312" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="AB48" s="312"/>
       <c r="AC48" s="312"/>
@@ -29576,7 +29565,7 @@
         <v>182</v>
       </c>
       <c r="C49" s="312" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D49" s="328"/>
       <c r="E49" s="328"/>
@@ -29588,7 +29577,7 @@
         <v>183</v>
       </c>
       <c r="K49" s="312" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="L49" s="312"/>
       <c r="M49" s="312"/>
@@ -29600,7 +29589,7 @@
         <v>184</v>
       </c>
       <c r="S49" s="312" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="T49" s="328"/>
       <c r="U49" s="328"/>
@@ -29612,7 +29601,7 @@
         <v>185</v>
       </c>
       <c r="AA49" s="312" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="AB49" s="312"/>
       <c r="AC49" s="312"/>
@@ -29626,7 +29615,7 @@
         <v>186</v>
       </c>
       <c r="C50" s="312" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D50" s="328"/>
       <c r="E50" s="328"/>
@@ -29638,7 +29627,7 @@
         <v>187</v>
       </c>
       <c r="K50" s="312" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="L50" s="312"/>
       <c r="M50" s="312"/>
@@ -29650,7 +29639,7 @@
         <v>188</v>
       </c>
       <c r="S50" s="312" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="T50" s="328"/>
       <c r="U50" s="328"/>
@@ -29662,7 +29651,7 @@
         <v>189</v>
       </c>
       <c r="AA50" s="312" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="AB50" s="312"/>
       <c r="AC50" s="312"/>
@@ -29676,7 +29665,7 @@
         <v>190</v>
       </c>
       <c r="C51" s="327" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D51" s="328"/>
       <c r="E51" s="328"/>
@@ -29688,7 +29677,7 @@
         <v>191</v>
       </c>
       <c r="K51" s="312" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="L51" s="312"/>
       <c r="M51" s="312"/>
@@ -29700,7 +29689,7 @@
         <v>192</v>
       </c>
       <c r="S51" s="327" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="T51" s="328"/>
       <c r="U51" s="328"/>
@@ -29712,7 +29701,7 @@
         <v>193</v>
       </c>
       <c r="AA51" s="312" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="AB51" s="312"/>
       <c r="AC51" s="312"/>
@@ -29726,7 +29715,7 @@
         <v>194</v>
       </c>
       <c r="C52" s="327" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D52" s="328"/>
       <c r="E52" s="328"/>
@@ -29738,7 +29727,7 @@
         <v>195</v>
       </c>
       <c r="K52" s="312" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="L52" s="312"/>
       <c r="M52" s="312"/>
@@ -29750,7 +29739,7 @@
         <v>196</v>
       </c>
       <c r="S52" s="327" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="T52" s="328"/>
       <c r="U52" s="328"/>
@@ -29762,7 +29751,7 @@
         <v>197</v>
       </c>
       <c r="AA52" s="312" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AB52" s="312"/>
       <c r="AC52" s="312"/>
@@ -29776,7 +29765,7 @@
         <v>198</v>
       </c>
       <c r="C53" s="327" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D53" s="328"/>
       <c r="E53" s="328"/>
@@ -29788,7 +29777,7 @@
         <v>199</v>
       </c>
       <c r="K53" s="312" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="L53" s="312"/>
       <c r="M53" s="312"/>
@@ -29800,7 +29789,7 @@
         <v>200</v>
       </c>
       <c r="S53" s="327" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="T53" s="328"/>
       <c r="U53" s="328"/>
@@ -29812,7 +29801,7 @@
         <v>201</v>
       </c>
       <c r="AA53" s="312" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="AB53" s="312"/>
       <c r="AC53" s="312"/>
@@ -29826,7 +29815,7 @@
         <v>202</v>
       </c>
       <c r="C54" s="327" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D54" s="328"/>
       <c r="E54" s="328"/>
@@ -29838,7 +29827,7 @@
         <v>203</v>
       </c>
       <c r="K54" s="312" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="L54" s="312"/>
       <c r="M54" s="312"/>
@@ -29850,7 +29839,7 @@
         <v>204</v>
       </c>
       <c r="S54" s="327" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="T54" s="328"/>
       <c r="U54" s="328"/>
@@ -29862,7 +29851,7 @@
         <v>205</v>
       </c>
       <c r="AA54" s="312" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="AB54" s="312"/>
       <c r="AC54" s="312"/>
@@ -29876,7 +29865,7 @@
         <v>206</v>
       </c>
       <c r="C55" s="327" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D55" s="328"/>
       <c r="E55" s="328"/>
@@ -29888,7 +29877,7 @@
         <v>207</v>
       </c>
       <c r="K55" s="312" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="L55" s="312"/>
       <c r="M55" s="312"/>
@@ -29900,7 +29889,7 @@
         <v>208</v>
       </c>
       <c r="S55" s="327" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="T55" s="328"/>
       <c r="U55" s="328"/>
@@ -29912,7 +29901,7 @@
         <v>209</v>
       </c>
       <c r="AA55" s="312" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="AB55" s="312"/>
       <c r="AC55" s="312"/>
@@ -29926,7 +29915,7 @@
         <v>210</v>
       </c>
       <c r="C56" s="327" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D56" s="328"/>
       <c r="E56" s="328"/>
@@ -29938,7 +29927,7 @@
         <v>211</v>
       </c>
       <c r="K56" s="312" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="L56" s="312"/>
       <c r="M56" s="312"/>
@@ -29950,7 +29939,7 @@
         <v>212</v>
       </c>
       <c r="S56" s="327" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="T56" s="328"/>
       <c r="U56" s="328"/>
@@ -29962,7 +29951,7 @@
         <v>213</v>
       </c>
       <c r="AA56" s="312" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="AB56" s="312"/>
       <c r="AC56" s="312"/>
@@ -29976,7 +29965,7 @@
         <v>214</v>
       </c>
       <c r="C57" s="327" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D57" s="328"/>
       <c r="E57" s="328"/>
@@ -29988,7 +29977,7 @@
         <v>215</v>
       </c>
       <c r="K57" s="312" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="L57" s="312"/>
       <c r="M57" s="312"/>
@@ -30000,7 +29989,7 @@
         <v>216</v>
       </c>
       <c r="S57" s="327" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="T57" s="328"/>
       <c r="U57" s="328"/>
@@ -30012,7 +30001,7 @@
         <v>217</v>
       </c>
       <c r="AA57" s="312" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="AB57" s="312"/>
       <c r="AC57" s="312"/>
@@ -30026,7 +30015,7 @@
         <v>218</v>
       </c>
       <c r="C58" s="327" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D58" s="328"/>
       <c r="E58" s="328"/>
@@ -30038,7 +30027,7 @@
         <v>219</v>
       </c>
       <c r="K58" s="312" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="L58" s="312"/>
       <c r="M58" s="312"/>
@@ -30050,7 +30039,7 @@
         <v>220</v>
       </c>
       <c r="S58" s="327" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="T58" s="328"/>
       <c r="U58" s="328"/>
@@ -30062,7 +30051,7 @@
         <v>221</v>
       </c>
       <c r="AA58" s="312" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="AB58" s="312"/>
       <c r="AC58" s="312"/>
@@ -30086,7 +30075,7 @@
         <v>223</v>
       </c>
       <c r="K59" s="312" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L59" s="312"/>
       <c r="M59" s="312"/>
@@ -30108,7 +30097,7 @@
         <v>225</v>
       </c>
       <c r="AA59" s="312" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="AB59" s="312"/>
       <c r="AC59" s="312"/>
@@ -30122,7 +30111,7 @@
         <v>226</v>
       </c>
       <c r="C60" s="312" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D60" s="312"/>
       <c r="E60" s="312"/>
@@ -30134,7 +30123,7 @@
         <v>227</v>
       </c>
       <c r="K60" s="312" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="L60" s="312"/>
       <c r="M60" s="312"/>
@@ -30156,7 +30145,7 @@
         <v>229</v>
       </c>
       <c r="AA60" s="312" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="AB60" s="312"/>
       <c r="AC60" s="312"/>
@@ -30170,7 +30159,7 @@
         <v>230</v>
       </c>
       <c r="C61" s="312" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D61" s="312"/>
       <c r="E61" s="312"/>
@@ -30182,7 +30171,7 @@
         <v>231</v>
       </c>
       <c r="K61" s="330" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="L61" s="331"/>
       <c r="M61" s="331"/>
@@ -30204,7 +30193,7 @@
         <v>233</v>
       </c>
       <c r="AA61" s="312" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AB61" s="312"/>
       <c r="AC61" s="312"/>
@@ -30218,7 +30207,7 @@
         <v>234</v>
       </c>
       <c r="C62" s="312" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D62" s="312"/>
       <c r="E62" s="312"/>
@@ -30230,7 +30219,7 @@
         <v>235</v>
       </c>
       <c r="K62" s="330" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="L62" s="331"/>
       <c r="M62" s="331"/>
@@ -30242,7 +30231,7 @@
         <v>236</v>
       </c>
       <c r="S62" s="320" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="T62" s="320"/>
       <c r="U62" s="320"/>
@@ -30254,7 +30243,7 @@
         <v>237</v>
       </c>
       <c r="AA62" s="312" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="AB62" s="312"/>
       <c r="AC62" s="312"/>
@@ -30299,7 +30288,7 @@
     </row>
     <row r="64" spans="2:33">
       <c r="B64" s="139" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="N64" s="178"/>
       <c r="O64" s="179"/>
@@ -30324,11 +30313,11 @@
     </row>
     <row r="65" spans="2:33">
       <c r="B65" s="333" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C65" s="334"/>
       <c r="D65" s="333" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E65" s="335"/>
       <c r="F65" s="335"/>
@@ -30336,11 +30325,11 @@
       <c r="H65" s="335"/>
       <c r="I65" s="334"/>
       <c r="J65" s="333" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="K65" s="334"/>
       <c r="L65" s="333" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="M65" s="335"/>
       <c r="N65" s="335"/>
@@ -30348,11 +30337,11 @@
       <c r="P65" s="335"/>
       <c r="Q65" s="334"/>
       <c r="R65" s="333" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="S65" s="334"/>
       <c r="T65" s="333" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="U65" s="335"/>
       <c r="V65" s="335"/>
@@ -30360,11 +30349,11 @@
       <c r="X65" s="335"/>
       <c r="Y65" s="334"/>
       <c r="Z65" s="333" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="AA65" s="334"/>
       <c r="AB65" s="333" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="AC65" s="335"/>
       <c r="AD65" s="335"/>
@@ -30378,7 +30367,7 @@
       </c>
       <c r="C66" s="336"/>
       <c r="D66" s="337" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E66" s="337"/>
       <c r="F66" s="337"/>
@@ -30390,7 +30379,7 @@
       </c>
       <c r="K66" s="336"/>
       <c r="L66" s="337" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="M66" s="337"/>
       <c r="N66" s="337"/>
@@ -30402,7 +30391,7 @@
       </c>
       <c r="S66" s="336"/>
       <c r="T66" s="337" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="U66" s="337"/>
       <c r="V66" s="337"/>
@@ -30414,7 +30403,7 @@
       </c>
       <c r="AA66" s="336"/>
       <c r="AB66" s="337" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="AC66" s="337"/>
       <c r="AD66" s="337"/>
@@ -30512,7 +30501,7 @@
       </c>
       <c r="C69" s="336"/>
       <c r="D69" s="337" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E69" s="337"/>
       <c r="F69" s="337"/>
@@ -30524,7 +30513,7 @@
       </c>
       <c r="K69" s="336"/>
       <c r="L69" s="337" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="M69" s="337"/>
       <c r="N69" s="337"/>
@@ -30536,7 +30525,7 @@
       </c>
       <c r="S69" s="336"/>
       <c r="T69" s="337" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="U69" s="337"/>
       <c r="V69" s="337"/>
@@ -30548,7 +30537,7 @@
       </c>
       <c r="AA69" s="336"/>
       <c r="AB69" s="337" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="AC69" s="337"/>
       <c r="AD69" s="337"/>
@@ -30646,7 +30635,7 @@
       </c>
       <c r="C72" s="336"/>
       <c r="D72" s="337" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E72" s="337"/>
       <c r="F72" s="337"/>
@@ -30668,7 +30657,7 @@
       </c>
       <c r="S72" s="336"/>
       <c r="T72" s="337" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="U72" s="337"/>
       <c r="V72" s="337"/>
@@ -30907,7 +30896,7 @@
       </c>
       <c r="K79" s="340"/>
       <c r="L79" s="341" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="M79" s="341"/>
       <c r="N79" s="341"/>
@@ -30927,7 +30916,7 @@
       </c>
       <c r="AA79" s="340"/>
       <c r="AB79" s="341" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="AC79" s="341"/>
       <c r="AD79" s="341"/>
@@ -31410,7 +31399,7 @@
       <c r="P2" s="259"/>
       <c r="Q2" s="140"/>
       <c r="R2" s="260" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S2" s="260"/>
       <c r="T2" s="260"/>
@@ -31437,14 +31426,14 @@
     <row r="3" spans="2:33" ht="23.5">
       <c r="C3" s="143"/>
       <c r="N3" s="240" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="R3" s="241"/>
       <c r="S3" s="241"/>
       <c r="T3" s="241"/>
       <c r="U3" s="241"/>
       <c r="V3" s="261" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="W3" s="261"/>
       <c r="X3" s="261"/>
@@ -31479,7 +31468,7 @@
     </row>
     <row r="5" spans="2:33" s="146" customFormat="1">
       <c r="B5" s="146" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D5" s="166"/>
       <c r="E5" s="166"/>
@@ -31512,10 +31501,10 @@
     </row>
     <row r="6" spans="2:33">
       <c r="B6" s="233" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C6" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D6" s="310"/>
       <c r="E6" s="310"/>
@@ -31524,10 +31513,10 @@
       <c r="H6" s="310"/>
       <c r="I6" s="310"/>
       <c r="J6" s="233" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K6" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="L6" s="310"/>
       <c r="M6" s="310"/>
@@ -31536,10 +31525,10 @@
       <c r="P6" s="310"/>
       <c r="Q6" s="310"/>
       <c r="R6" s="236" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="S6" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="T6" s="310"/>
       <c r="U6" s="310"/>
@@ -31548,10 +31537,10 @@
       <c r="X6" s="310"/>
       <c r="Y6" s="310"/>
       <c r="Z6" s="236" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="AA6" s="310" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="AB6" s="310"/>
       <c r="AC6" s="310"/>
@@ -31565,7 +31554,7 @@
         <v>109</v>
       </c>
       <c r="C7" s="317" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D7" s="317"/>
       <c r="E7" s="317"/>
@@ -31603,7 +31592,7 @@
         <v>493</v>
       </c>
       <c r="C8" s="330" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D8" s="331"/>
       <c r="E8" s="331"/>
@@ -31625,7 +31614,7 @@
         <v>259</v>
       </c>
       <c r="S8" s="330" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="T8" s="331"/>
       <c r="U8" s="331"/>
@@ -31649,7 +31638,7 @@
         <v>261</v>
       </c>
       <c r="C9" s="330" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D9" s="331"/>
       <c r="E9" s="331"/>
@@ -31671,7 +31660,7 @@
         <v>262</v>
       </c>
       <c r="S9" s="330" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="T9" s="331"/>
       <c r="U9" s="331"/>
@@ -31695,7 +31684,7 @@
         <v>264</v>
       </c>
       <c r="C10" s="330" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D10" s="331"/>
       <c r="E10" s="331"/>
@@ -31717,7 +31706,7 @@
         <v>266</v>
       </c>
       <c r="S10" s="330" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="T10" s="331"/>
       <c r="U10" s="331"/>
@@ -31741,7 +31730,7 @@
         <v>268</v>
       </c>
       <c r="C11" s="330" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D11" s="331"/>
       <c r="E11" s="331"/>
@@ -31763,7 +31752,7 @@
         <v>270</v>
       </c>
       <c r="S11" s="330" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="T11" s="331"/>
       <c r="U11" s="331"/>
@@ -31787,7 +31776,7 @@
         <v>272</v>
       </c>
       <c r="C12" s="330" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D12" s="331"/>
       <c r="E12" s="331"/>
@@ -31809,7 +31798,7 @@
         <v>274</v>
       </c>
       <c r="S12" s="330" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="T12" s="331"/>
       <c r="U12" s="331"/>
@@ -31833,7 +31822,7 @@
         <v>276</v>
       </c>
       <c r="C13" s="330" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D13" s="331"/>
       <c r="E13" s="331"/>
@@ -31855,7 +31844,7 @@
         <v>278</v>
       </c>
       <c r="S13" s="330" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="T13" s="331"/>
       <c r="U13" s="331"/>
@@ -31879,7 +31868,7 @@
         <v>280</v>
       </c>
       <c r="C14" s="330" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D14" s="331"/>
       <c r="E14" s="331"/>
@@ -31901,7 +31890,7 @@
         <v>282</v>
       </c>
       <c r="S14" s="330" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="T14" s="331"/>
       <c r="U14" s="331"/>
@@ -31925,7 +31914,7 @@
         <v>284</v>
       </c>
       <c r="C15" s="330" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D15" s="331"/>
       <c r="E15" s="331"/>
@@ -31947,7 +31936,7 @@
         <v>286</v>
       </c>
       <c r="S15" s="330" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="T15" s="331"/>
       <c r="U15" s="331"/>
@@ -31971,7 +31960,7 @@
         <v>288</v>
       </c>
       <c r="C16" s="330" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D16" s="331"/>
       <c r="E16" s="331"/>
@@ -31993,7 +31982,7 @@
         <v>290</v>
       </c>
       <c r="S16" s="330" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="T16" s="331"/>
       <c r="U16" s="331"/>
@@ -32017,7 +32006,7 @@
         <v>292</v>
       </c>
       <c r="C17" s="330" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D17" s="331"/>
       <c r="E17" s="331"/>
@@ -32039,7 +32028,7 @@
         <v>294</v>
       </c>
       <c r="S17" s="330" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="T17" s="331"/>
       <c r="U17" s="331"/>
@@ -32063,7 +32052,7 @@
         <v>296</v>
       </c>
       <c r="C18" s="330" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D18" s="331"/>
       <c r="E18" s="331"/>
@@ -32085,7 +32074,7 @@
         <v>298</v>
       </c>
       <c r="S18" s="330" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="T18" s="331"/>
       <c r="U18" s="331"/>
@@ -32109,7 +32098,7 @@
         <v>300</v>
       </c>
       <c r="C19" s="330" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D19" s="331"/>
       <c r="E19" s="331"/>
@@ -32131,7 +32120,7 @@
         <v>302</v>
       </c>
       <c r="S19" s="330" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="T19" s="331"/>
       <c r="U19" s="331"/>
@@ -32155,7 +32144,7 @@
         <v>304</v>
       </c>
       <c r="C20" s="330" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D20" s="331"/>
       <c r="E20" s="331"/>
@@ -32177,7 +32166,7 @@
         <v>306</v>
       </c>
       <c r="S20" s="330" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="T20" s="331"/>
       <c r="U20" s="331"/>
@@ -32201,7 +32190,7 @@
         <v>308</v>
       </c>
       <c r="C21" s="330" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D21" s="331"/>
       <c r="E21" s="331"/>
@@ -32223,7 +32212,7 @@
         <v>310</v>
       </c>
       <c r="S21" s="330" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="T21" s="331"/>
       <c r="U21" s="331"/>
@@ -32247,7 +32236,7 @@
         <v>255</v>
       </c>
       <c r="C22" s="330" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D22" s="331"/>
       <c r="E22" s="331"/>
@@ -32269,7 +32258,7 @@
         <v>313</v>
       </c>
       <c r="S22" s="330" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="T22" s="331"/>
       <c r="U22" s="331"/>
@@ -32293,7 +32282,7 @@
         <v>315</v>
       </c>
       <c r="C23" s="330" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D23" s="331"/>
       <c r="E23" s="331"/>
@@ -32315,7 +32304,7 @@
         <v>316</v>
       </c>
       <c r="S23" s="330" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="T23" s="331"/>
       <c r="U23" s="331"/>
@@ -32339,7 +32328,7 @@
         <v>318</v>
       </c>
       <c r="C24" s="330" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D24" s="331"/>
       <c r="E24" s="331"/>
@@ -32361,7 +32350,7 @@
         <v>320</v>
       </c>
       <c r="S24" s="330" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="T24" s="331"/>
       <c r="U24" s="331"/>
@@ -32385,7 +32374,7 @@
         <v>322</v>
       </c>
       <c r="C25" s="330" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D25" s="331"/>
       <c r="E25" s="331"/>
@@ -32407,7 +32396,7 @@
         <v>324</v>
       </c>
       <c r="S25" s="330" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="T25" s="331"/>
       <c r="U25" s="331"/>
@@ -32431,7 +32420,7 @@
         <v>326</v>
       </c>
       <c r="C26" s="330" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D26" s="331"/>
       <c r="E26" s="331"/>
@@ -32453,7 +32442,7 @@
         <v>328</v>
       </c>
       <c r="S26" s="330" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="T26" s="331"/>
       <c r="U26" s="331"/>
@@ -32477,7 +32466,7 @@
         <v>330</v>
       </c>
       <c r="C27" s="330" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D27" s="331"/>
       <c r="E27" s="331"/>
@@ -32499,7 +32488,7 @@
         <v>332</v>
       </c>
       <c r="S27" s="330" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="T27" s="331"/>
       <c r="U27" s="331"/>
@@ -32523,7 +32512,7 @@
         <v>334</v>
       </c>
       <c r="C28" s="330" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D28" s="331"/>
       <c r="E28" s="331"/>
@@ -32535,7 +32524,7 @@
         <v>335</v>
       </c>
       <c r="K28" s="330" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="L28" s="331"/>
       <c r="M28" s="331"/>
@@ -32547,7 +32536,7 @@
         <v>336</v>
       </c>
       <c r="S28" s="330" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="T28" s="331"/>
       <c r="U28" s="331"/>
@@ -32559,7 +32548,7 @@
         <v>337</v>
       </c>
       <c r="AA28" s="330" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="AB28" s="331"/>
       <c r="AC28" s="331"/>
@@ -32573,7 +32562,7 @@
         <v>338</v>
       </c>
       <c r="C29" s="330" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D29" s="331"/>
       <c r="E29" s="331"/>
@@ -32585,7 +32574,7 @@
         <v>339</v>
       </c>
       <c r="K29" s="330" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="L29" s="331"/>
       <c r="M29" s="331"/>
@@ -32597,7 +32586,7 @@
         <v>340</v>
       </c>
       <c r="S29" s="330" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="T29" s="331"/>
       <c r="U29" s="331"/>
@@ -32609,7 +32598,7 @@
         <v>341</v>
       </c>
       <c r="AA29" s="342" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="AB29" s="343"/>
       <c r="AC29" s="343"/>
@@ -32623,7 +32612,7 @@
         <v>342</v>
       </c>
       <c r="C30" s="330" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D30" s="331"/>
       <c r="E30" s="331"/>
@@ -32635,7 +32624,7 @@
         <v>343</v>
       </c>
       <c r="K30" s="330" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="L30" s="331"/>
       <c r="M30" s="331"/>
@@ -32647,7 +32636,7 @@
         <v>344</v>
       </c>
       <c r="S30" s="330" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="T30" s="331"/>
       <c r="U30" s="331"/>
@@ -32659,7 +32648,7 @@
         <v>345</v>
       </c>
       <c r="AA30" s="342" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="AB30" s="343"/>
       <c r="AC30" s="343"/>
@@ -32673,7 +32662,7 @@
         <v>346</v>
       </c>
       <c r="C31" s="330" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D31" s="331"/>
       <c r="E31" s="331"/>
@@ -32685,7 +32674,7 @@
         <v>347</v>
       </c>
       <c r="K31" s="330" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="L31" s="331"/>
       <c r="M31" s="331"/>
@@ -32697,7 +32686,7 @@
         <v>348</v>
       </c>
       <c r="S31" s="330" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="T31" s="331"/>
       <c r="U31" s="331"/>
@@ -32709,7 +32698,7 @@
         <v>349</v>
       </c>
       <c r="AA31" s="342" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="AB31" s="343"/>
       <c r="AC31" s="343"/>
@@ -32723,7 +32712,7 @@
         <v>350</v>
       </c>
       <c r="C32" s="330" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D32" s="331"/>
       <c r="E32" s="331"/>
@@ -32735,7 +32724,7 @@
         <v>351</v>
       </c>
       <c r="K32" s="330" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="L32" s="331"/>
       <c r="M32" s="331"/>
@@ -32747,7 +32736,7 @@
         <v>352</v>
       </c>
       <c r="S32" s="330" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="T32" s="331"/>
       <c r="U32" s="331"/>
@@ -32759,7 +32748,7 @@
         <v>353</v>
       </c>
       <c r="AA32" s="342" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="AB32" s="343"/>
       <c r="AC32" s="343"/>
@@ -32773,7 +32762,7 @@
         <v>354</v>
       </c>
       <c r="C33" s="330" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D33" s="331"/>
       <c r="E33" s="331"/>
@@ -32785,7 +32774,7 @@
         <v>355</v>
       </c>
       <c r="K33" s="330" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="L33" s="331"/>
       <c r="M33" s="331"/>
@@ -32797,7 +32786,7 @@
         <v>356</v>
       </c>
       <c r="S33" s="330" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="T33" s="331"/>
       <c r="U33" s="331"/>
@@ -32809,7 +32798,7 @@
         <v>357</v>
       </c>
       <c r="AA33" s="342" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="AB33" s="343"/>
       <c r="AC33" s="343"/>
@@ -32823,7 +32812,7 @@
         <v>358</v>
       </c>
       <c r="C34" s="330" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D34" s="331"/>
       <c r="E34" s="331"/>
@@ -32835,7 +32824,7 @@
         <v>359</v>
       </c>
       <c r="K34" s="330" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="L34" s="331"/>
       <c r="M34" s="331"/>
@@ -32847,7 +32836,7 @@
         <v>360</v>
       </c>
       <c r="S34" s="330" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="T34" s="331"/>
       <c r="U34" s="331"/>
@@ -32859,7 +32848,7 @@
         <v>361</v>
       </c>
       <c r="AA34" s="342" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="AB34" s="343"/>
       <c r="AC34" s="343"/>
@@ -32873,7 +32862,7 @@
         <v>362</v>
       </c>
       <c r="C35" s="330" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D35" s="331"/>
       <c r="E35" s="331"/>
@@ -32885,7 +32874,7 @@
         <v>363</v>
       </c>
       <c r="K35" s="330" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="L35" s="331"/>
       <c r="M35" s="331"/>
@@ -32897,7 +32886,7 @@
         <v>364</v>
       </c>
       <c r="S35" s="330" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="T35" s="331"/>
       <c r="U35" s="331"/>
@@ -32909,7 +32898,7 @@
         <v>365</v>
       </c>
       <c r="AA35" s="342" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="AB35" s="343"/>
       <c r="AC35" s="343"/>
@@ -32923,7 +32912,7 @@
         <v>366</v>
       </c>
       <c r="C36" s="330" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D36" s="331"/>
       <c r="E36" s="331"/>
@@ -32935,7 +32924,7 @@
         <v>367</v>
       </c>
       <c r="K36" s="330" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="L36" s="331"/>
       <c r="M36" s="331"/>
@@ -32947,7 +32936,7 @@
         <v>368</v>
       </c>
       <c r="S36" s="330" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="T36" s="331"/>
       <c r="U36" s="331"/>
@@ -32959,7 +32948,7 @@
         <v>369</v>
       </c>
       <c r="AA36" s="330" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="AB36" s="331"/>
       <c r="AC36" s="331"/>
@@ -32973,7 +32962,7 @@
         <v>370</v>
       </c>
       <c r="C37" s="330" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D37" s="331"/>
       <c r="E37" s="331"/>
@@ -32985,7 +32974,7 @@
         <v>371</v>
       </c>
       <c r="K37" s="330" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="L37" s="331"/>
       <c r="M37" s="331"/>
@@ -32997,7 +32986,7 @@
         <v>372</v>
       </c>
       <c r="S37" s="330" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="T37" s="331"/>
       <c r="U37" s="331"/>
@@ -33009,7 +32998,7 @@
         <v>373</v>
       </c>
       <c r="AA37" s="330" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="AB37" s="331"/>
       <c r="AC37" s="331"/>
@@ -33023,7 +33012,7 @@
         <v>374</v>
       </c>
       <c r="C38" s="330" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D38" s="331"/>
       <c r="E38" s="331"/>
@@ -33035,7 +33024,7 @@
         <v>375</v>
       </c>
       <c r="K38" s="330" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="L38" s="331"/>
       <c r="M38" s="331"/>
@@ -33047,7 +33036,7 @@
         <v>376</v>
       </c>
       <c r="S38" s="330" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="T38" s="331"/>
       <c r="U38" s="331"/>
@@ -33059,7 +33048,7 @@
         <v>377</v>
       </c>
       <c r="AA38" s="330" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="AB38" s="331"/>
       <c r="AC38" s="331"/>
@@ -33073,7 +33062,7 @@
         <v>378</v>
       </c>
       <c r="C39" s="330" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D39" s="331"/>
       <c r="E39" s="331"/>
@@ -33085,7 +33074,7 @@
         <v>379</v>
       </c>
       <c r="K39" s="330" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="L39" s="331"/>
       <c r="M39" s="331"/>
@@ -33097,7 +33086,7 @@
         <v>380</v>
       </c>
       <c r="S39" s="330" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="T39" s="331"/>
       <c r="U39" s="331"/>
@@ -33109,7 +33098,7 @@
         <v>381</v>
       </c>
       <c r="AA39" s="330" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="AB39" s="331"/>
       <c r="AC39" s="331"/>
@@ -33133,7 +33122,7 @@
         <v>383</v>
       </c>
       <c r="K40" s="330" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="L40" s="331"/>
       <c r="M40" s="331"/>
@@ -33155,7 +33144,7 @@
         <v>385</v>
       </c>
       <c r="AA40" s="330" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="AB40" s="331"/>
       <c r="AC40" s="331"/>
@@ -33179,7 +33168,7 @@
         <v>387</v>
       </c>
       <c r="K41" s="330" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="L41" s="331"/>
       <c r="M41" s="331"/>
@@ -33201,7 +33190,7 @@
         <v>389</v>
       </c>
       <c r="AA41" s="330" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="AB41" s="331"/>
       <c r="AC41" s="331"/>
@@ -33225,7 +33214,7 @@
         <v>391</v>
       </c>
       <c r="K42" s="330" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="L42" s="331"/>
       <c r="M42" s="331"/>
@@ -33247,7 +33236,7 @@
         <v>393</v>
       </c>
       <c r="AA42" s="330" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="AB42" s="331"/>
       <c r="AC42" s="331"/>
@@ -33271,7 +33260,7 @@
         <v>395</v>
       </c>
       <c r="K43" s="330" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="L43" s="331"/>
       <c r="M43" s="331"/>
@@ -33293,7 +33282,7 @@
         <v>397</v>
       </c>
       <c r="AA43" s="330" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="AB43" s="331"/>
       <c r="AC43" s="331"/>
@@ -33317,7 +33306,7 @@
         <v>399</v>
       </c>
       <c r="K44" s="330" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="L44" s="331"/>
       <c r="M44" s="331"/>
@@ -33339,7 +33328,7 @@
         <v>401</v>
       </c>
       <c r="AA44" s="330" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="AB44" s="331"/>
       <c r="AC44" s="331"/>
@@ -33363,7 +33352,7 @@
         <v>403</v>
       </c>
       <c r="K45" s="330" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="L45" s="331"/>
       <c r="M45" s="331"/>
@@ -33385,7 +33374,7 @@
         <v>405</v>
       </c>
       <c r="AA45" s="330" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="AB45" s="331"/>
       <c r="AC45" s="331"/>
@@ -33409,7 +33398,7 @@
         <v>407</v>
       </c>
       <c r="K46" s="330" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="L46" s="331"/>
       <c r="M46" s="331"/>
@@ -33431,7 +33420,7 @@
         <v>409</v>
       </c>
       <c r="AA46" s="330" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="AB46" s="331"/>
       <c r="AC46" s="331"/>
@@ -33455,7 +33444,7 @@
         <v>411</v>
       </c>
       <c r="K47" s="330" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="L47" s="331"/>
       <c r="M47" s="331"/>
@@ -33477,7 +33466,7 @@
         <v>413</v>
       </c>
       <c r="AA47" s="330" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="AB47" s="331"/>
       <c r="AC47" s="331"/>
@@ -33501,7 +33490,7 @@
         <v>415</v>
       </c>
       <c r="K48" s="330" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="L48" s="331"/>
       <c r="M48" s="331"/>
@@ -33523,7 +33512,7 @@
         <v>417</v>
       </c>
       <c r="AA48" s="330" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="AB48" s="331"/>
       <c r="AC48" s="331"/>
@@ -33547,7 +33536,7 @@
         <v>419</v>
       </c>
       <c r="K49" s="330" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="L49" s="331"/>
       <c r="M49" s="331"/>
@@ -33569,7 +33558,7 @@
         <v>421</v>
       </c>
       <c r="AA49" s="330" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="AB49" s="331"/>
       <c r="AC49" s="331"/>
@@ -33593,7 +33582,7 @@
         <v>423</v>
       </c>
       <c r="K50" s="330" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="L50" s="331"/>
       <c r="M50" s="331"/>
@@ -33615,7 +33604,7 @@
         <v>425</v>
       </c>
       <c r="AA50" s="330" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="AB50" s="331"/>
       <c r="AC50" s="331"/>
@@ -33639,7 +33628,7 @@
         <v>427</v>
       </c>
       <c r="K51" s="330" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="L51" s="331"/>
       <c r="M51" s="331"/>
@@ -33661,7 +33650,7 @@
         <v>429</v>
       </c>
       <c r="AA51" s="330" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="AB51" s="331"/>
       <c r="AC51" s="331"/>
@@ -33685,7 +33674,7 @@
         <v>431</v>
       </c>
       <c r="K52" s="330" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="L52" s="331"/>
       <c r="M52" s="331"/>
@@ -33707,7 +33696,7 @@
         <v>433</v>
       </c>
       <c r="AA52" s="330" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="AB52" s="331"/>
       <c r="AC52" s="331"/>
@@ -33731,7 +33720,7 @@
         <v>435</v>
       </c>
       <c r="K53" s="330" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="L53" s="331"/>
       <c r="M53" s="331"/>
@@ -33753,7 +33742,7 @@
         <v>437</v>
       </c>
       <c r="AA53" s="330" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="AB53" s="331"/>
       <c r="AC53" s="331"/>
@@ -33777,7 +33766,7 @@
         <v>439</v>
       </c>
       <c r="K54" s="330" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="L54" s="331"/>
       <c r="M54" s="331"/>
@@ -33799,7 +33788,7 @@
         <v>441</v>
       </c>
       <c r="AA54" s="330" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="AB54" s="331"/>
       <c r="AC54" s="331"/>
@@ -33823,7 +33812,7 @@
         <v>443</v>
       </c>
       <c r="K55" s="330" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="L55" s="331"/>
       <c r="M55" s="331"/>
@@ -33845,7 +33834,7 @@
         <v>445</v>
       </c>
       <c r="AA55" s="330" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="AB55" s="331"/>
       <c r="AC55" s="331"/>

</xml_diff>